<commit_message>
I modified Excel _ Test 1.xlsx file
</commit_message>
<xml_diff>
--- a/Exel _ Test 1.xlsx
+++ b/Exel _ Test 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GIT Tranining\GIT Hub\alemrepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF2BB79-87FE-437F-9B09-6CD6B2063F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBD3611-E161-46F3-8144-DC4698937282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>No.</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>Country</t>
+  </si>
+  <si>
+    <t>wondifraw</t>
+  </si>
+  <si>
+    <t>nigussie</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>ethiopia</t>
   </si>
 </sst>
 </file>
@@ -382,10 +394,13 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -411,13 +426,27 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1">
+        <v>45</v>
+      </c>
+      <c r="E2" s="1">
+        <v>911513683</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>

</xml_diff>